<commit_message>
[GRE] Revisão 2 de requisitos funcionais realizada.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Revisão 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Legenda" sheetId="2" r:id="rId2"/>
+    <sheet name="Revisão 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Legenda" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="24">
   <si>
     <t>Sigla do Requisito</t>
   </si>
@@ -66,6 +67,27 @@
   </si>
   <si>
     <t>RFUN2.4</t>
+  </si>
+  <si>
+    <t>RFUN3.1</t>
+  </si>
+  <si>
+    <t>RFUN3.2</t>
+  </si>
+  <si>
+    <t>RFUN3.3</t>
+  </si>
+  <si>
+    <t>RFUN4.1</t>
+  </si>
+  <si>
+    <t>RFUN4.2</t>
+  </si>
+  <si>
+    <t>RFUN4.3</t>
+  </si>
+  <si>
+    <t>RFUN4.4</t>
   </si>
 </sst>
 </file>
@@ -439,13 +461,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:K9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="2" max="11" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -771,10 +792,273 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[GRE] Revisão 3 de requisitos funcionais realizada.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Revisão 1" sheetId="1" r:id="rId1"/>
     <sheet name="Revisão 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Legenda" sheetId="2" r:id="rId3"/>
+    <sheet name="Revisão 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Legenda" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="32">
   <si>
     <t>Sigla do Requisito</t>
   </si>
@@ -88,6 +89,30 @@
   </si>
   <si>
     <t>RFUN4.4</t>
+  </si>
+  <si>
+    <t>RFUN5.1</t>
+  </si>
+  <si>
+    <t>RFUN5.2</t>
+  </si>
+  <si>
+    <t>RFUN5.3</t>
+  </si>
+  <si>
+    <t>RFUN5.4</t>
+  </si>
+  <si>
+    <t>RFUN5.5</t>
+  </si>
+  <si>
+    <t>RFUN6.1</t>
+  </si>
+  <si>
+    <t>RFUN6.2</t>
+  </si>
+  <si>
+    <t>RFUN6.3</t>
   </si>
 </sst>
 </file>
@@ -794,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -1054,6 +1079,304 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
[GRE] Realizando revisões 4, 5 e 6 de requisitos
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Revisão 1" sheetId="1" r:id="rId1"/>
     <sheet name="Revisão 2" sheetId="3" r:id="rId2"/>
     <sheet name="Revisão 3" sheetId="4" r:id="rId3"/>
-    <sheet name="Legenda" sheetId="2" r:id="rId4"/>
+    <sheet name="Revisão 4" sheetId="5" r:id="rId4"/>
+    <sheet name="Revisão 5" sheetId="7" r:id="rId5"/>
+    <sheet name="Revisão 6" sheetId="8" r:id="rId6"/>
+    <sheet name="Legenda" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="53">
   <si>
     <t>Sigla do Requisito</t>
   </si>
@@ -113,6 +116,69 @@
   </si>
   <si>
     <t>RFUN6.3</t>
+  </si>
+  <si>
+    <t>RFUN7.5</t>
+  </si>
+  <si>
+    <t>RFUN7.4</t>
+  </si>
+  <si>
+    <t>RFUN7.3</t>
+  </si>
+  <si>
+    <t>RFUN7.2</t>
+  </si>
+  <si>
+    <t>RFUN7.1</t>
+  </si>
+  <si>
+    <t>RFUN8.1</t>
+  </si>
+  <si>
+    <t>RFUN8.2</t>
+  </si>
+  <si>
+    <t>RFUN9.1</t>
+  </si>
+  <si>
+    <t>RFUN9.2</t>
+  </si>
+  <si>
+    <t>RFUN9.3</t>
+  </si>
+  <si>
+    <t>RFUN9.4</t>
+  </si>
+  <si>
+    <t>RFUN9.5</t>
+  </si>
+  <si>
+    <t>RFUN9.6</t>
+  </si>
+  <si>
+    <t>RFUN9.7</t>
+  </si>
+  <si>
+    <t>RFUN11.1</t>
+  </si>
+  <si>
+    <t>RFUN11.2</t>
+  </si>
+  <si>
+    <t>RFUN10.1</t>
+  </si>
+  <si>
+    <t>RFUN10.2</t>
+  </si>
+  <si>
+    <t>RFUN10.3</t>
+  </si>
+  <si>
+    <t>RFUN10.4</t>
+  </si>
+  <si>
+    <t>RFUN10.5</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1377,6 +1443,834 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
[GRE] Atualizando DVR e RR para melhor adequação ao GRE/MPS.BR Nível G
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Revisões de Requisitos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Revisão 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="54">
   <si>
     <t>Sigla do Requisito</t>
   </si>
@@ -28,18 +28,6 @@
     <t>Sim/Não</t>
   </si>
   <si>
-    <t>Abreviação e Número</t>
-  </si>
-  <si>
-    <t>Resposta da Questão*</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A numeração de uma questão é de modo que a coluna 'B' refere-se à questão 'a' do PRR e assim sucessivamente até que a coluna 'K' finalize o agrupamento das respostas com a resposta da questão 'j'.</t>
-  </si>
-  <si>
-    <t>Obs: As questões referenciadas neste documento de revisão estão documentadas no plano de revisão de requisitos (PRR).</t>
-  </si>
-  <si>
     <t>RFUN1.1</t>
   </si>
   <si>
@@ -179,6 +167,21 @@
   </si>
   <si>
     <t>RFUN10.5</t>
+  </si>
+  <si>
+    <t>Resposta da Questão</t>
+  </si>
+  <si>
+    <t>Abreviação e Número*</t>
+  </si>
+  <si>
+    <t>Obs: As questões referenciadas (e suas respectivas respostas esperadas) neste documento estão documentadas no plano de revisão de requisitos (PRR).</t>
+  </si>
+  <si>
+    <t>* O número de um requisito tem o seguinte modelo: X.Y    X representa o caso de uso ao qual ele pertence e Y representa a numeração deste requisito dentro deste caso de uso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A numeração de uma questão é descrita de modo tal que a coluna 'B' refere-se à questão 'a' do PRR e assim sucessivamente até que a coluna 'K' que contém a resposta da questão 'j'.</t>
   </si>
 </sst>
 </file>
@@ -562,317 +565,317 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -896,247 +899,247 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1159,282 +1162,282 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1457,247 +1460,247 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1733,247 +1736,247 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1998,7 +2001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -2009,247 +2012,247 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2272,47 +2275,51 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
+    <row r="4" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="Obs: As questões referenciadas neste documento de revisão estão documentadas no plano de revisão de requisitos (PRR)"/>
+    <hyperlink ref="C4" r:id="rId1" display="Obs: As questões referenciadas neste documento de revisão estão documentadas no plano de revisão de requisitos (PRR)"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>